<commit_message>
Sprint 10 update day 4
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint10.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint10.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -860,40 +860,40 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,11 +914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="213831848"/>
-        <c:axId val="213824400"/>
+        <c:axId val="286941984"/>
+        <c:axId val="286942376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213831848"/>
+        <c:axId val="286941984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213824400"/>
+        <c:crossAx val="286942376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1029,7 +1029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213824400"/>
+        <c:axId val="286942376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213831848"/>
+        <c:crossAx val="286941984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1795,7 +1795,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2200,7 +2200,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2527,11 +2527,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -2545,7 +2547,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -2554,16 +2556,20 @@
       <c r="C12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -2577,7 +2583,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -2586,12 +2592,14 @@
       <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E13" s="2">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2773,7 +2781,7 @@
       </c>
       <c r="I18" s="2">
         <f t="shared" ref="I18:T18" si="2">SUM(I5:I17)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="2"/>
@@ -2821,7 +2829,7 @@
       </c>
       <c r="U18" s="2">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -2916,51 +2924,51 @@
       </c>
       <c r="I20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="S20" s="2">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="T20" s="2">
         <f>S20-SUM(T5:T17)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U20" s="10"/>
     </row>

</xml_diff>

<commit_message>
Added info to Sprint10
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint10.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint10.xlsx
@@ -473,22 +473,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="0"/>
@@ -906,10 +891,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,11 +915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="283384296"/>
-        <c:axId val="283384688"/>
+        <c:axId val="290805320"/>
+        <c:axId val="290807280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="283384296"/>
+        <c:axId val="290805320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283384688"/>
+        <c:crossAx val="290807280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1045,7 +1030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283384688"/>
+        <c:axId val="290807280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283384296"/>
+        <c:crossAx val="290805320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1812,7 +1797,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2217,7 +2202,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2406,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2420,11 +2405,13 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -2856,7 +2843,7 @@
       </c>
       <c r="S18" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="2">
         <f t="shared" si="2"/>
@@ -2864,7 +2851,7 @@
       </c>
       <c r="U18" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -2999,11 +2986,11 @@
       </c>
       <c r="S20" s="2">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T20" s="2">
         <f>S20-SUM(T5:T17)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U20" s="10"/>
     </row>
@@ -3049,28 +3036,28 @@
     <mergeCell ref="B11:B14"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F17">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U7 U15:U18">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:U10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:U14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Small change to Sprint info 10 and 11
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint10.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint10.xlsx
@@ -578,7 +578,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -915,11 +914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="290805320"/>
-        <c:axId val="290807280"/>
+        <c:axId val="272201824"/>
+        <c:axId val="272203000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290805320"/>
+        <c:axId val="272201824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290807280"/>
+        <c:crossAx val="272203000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1030,7 +1029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290807280"/>
+        <c:axId val="272203000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1074,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1134,7 +1132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290805320"/>
+        <c:crossAx val="272201824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,7 +1795,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2202,7 +2200,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2543,13 +2541,11 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -2563,7 +2559,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -2615,11 +2611,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -2633,7 +2631,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>